<commit_message>
Toutes les combinaisons d'hyperparamètres ont été testées pour deep_network, y compris (-0.1, 0.1) !
</commit_message>
<xml_diff>
--- a/excel/deep_network_combinaison.xlsx
+++ b/excel/deep_network_combinaison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasse\Desktop\cours\5A\Deep learning\deep_learning_lefort\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E639478-019F-4F31-A7BA-C8A5753918A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87963329-1161-4AE6-BDBA-9B4E369BB239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A913" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F961" sqref="F961"/>
+    <sheetView tabSelected="1" topLeftCell="A369" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5703125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
il manque les commentaires
</commit_message>
<xml_diff>
--- a/excel/deep_network_combinaison.xlsx
+++ b/excel/deep_network_combinaison.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasse\Desktop\cours\5A\Deep learning\deep_learning_lefort\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49167FE6-5C36-4526-8E42-F8268F2B396A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432C9D50-617A-4B75-B340-18C4068B0490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="EVERYTHING" sheetId="2" r:id="rId2"/>
+    <sheet name="EVERYTHING" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -438,23 +437,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1171" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1047" sqref="J1047"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5703125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>